<commit_message>
- implememt search and get features - term recognition is now showing results from the excel term provider
</commit_message>
<xml_diff>
--- a/Sdl.Community.ExcelTerminology/Sdl.Community.ExcelTerminology.Tests/Resources/glossary_example.xlsx
+++ b/Sdl.Community.ExcelTerminology/Sdl.Community.ExcelTerminology.Tests/Resources/glossary_example.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pfilkin\Documents\SDL\Development\OpenExchange\Excel Terminology Provider\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Git\Sdl-Community\Sdl.Community.ExcelTerminology\Sdl.Community.ExcelTerminology.Tests\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="8220"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15336" windowHeight="8220"/>
   </bookViews>
   <sheets>
     <sheet name="Glossary" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="70">
   <si>
     <t>abeyance</t>
   </si>
@@ -193,12 +193,48 @@
   </si>
   <si>
     <t>Approved|Not approved|Approved|Approved</t>
+  </si>
+  <si>
+    <t>getting</t>
+  </si>
+  <si>
+    <t>erste</t>
+  </si>
+  <si>
+    <t>Not approved</t>
+  </si>
+  <si>
+    <t>finding</t>
+  </si>
+  <si>
+    <t>Geeigneten</t>
+  </si>
+  <si>
+    <t>register</t>
+  </si>
+  <si>
+    <t>registrieren|anmelden</t>
+  </si>
+  <si>
+    <t>Approved|Approved</t>
+  </si>
+  <si>
+    <t>obtain</t>
+  </si>
+  <si>
+    <t>erhalten</t>
+  </si>
+  <si>
+    <t>discount</t>
+  </si>
+  <si>
+    <t>Rabatt|Diskont</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -983,20 +1019,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>52</v>
       </c>
@@ -1007,7 +1043,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1018,7 +1054,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1029,7 +1065,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1040,7 +1076,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1051,7 +1087,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1062,7 +1098,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1073,7 +1109,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1084,7 +1120,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1095,7 +1131,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1106,7 +1142,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1117,7 +1153,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1128,7 +1164,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1139,7 +1175,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1150,7 +1186,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1161,7 +1197,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1172,7 +1208,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1183,7 +1219,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1194,7 +1230,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -1205,7 +1241,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -1216,7 +1252,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -1227,7 +1263,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -1238,7 +1274,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -1249,7 +1285,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -1260,7 +1296,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -1271,7 +1307,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -1282,7 +1318,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>50</v>
       </c>
@@ -1291,6 +1327,61 @@
       </c>
       <c r="C27" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>